<commit_message>
Work on ch 2
</commit_message>
<xml_diff>
--- a/data/misc.xlsx
+++ b/data/misc.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="28720" windowHeight="9480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="1320" windowWidth="28720" windowHeight="15400" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="tf list" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="76">
   <si>
     <t>zen</t>
   </si>
@@ -122,6 +123,138 @@
   </si>
   <si>
     <t>% of Protein-Coding Genome Differentially Expressed vs wild-type</t>
+  </si>
+  <si>
+    <t>bcd_1</t>
+  </si>
+  <si>
+    <t>bcd_2</t>
+  </si>
+  <si>
+    <t>cad_1</t>
+  </si>
+  <si>
+    <t>D_1</t>
+  </si>
+  <si>
+    <t>da_2</t>
+  </si>
+  <si>
+    <t>dl_3</t>
+  </si>
+  <si>
+    <t>ftz_3</t>
+  </si>
+  <si>
+    <t>gt_2</t>
+  </si>
+  <si>
+    <t>hb_1</t>
+  </si>
+  <si>
+    <t>hb_2</t>
+  </si>
+  <si>
+    <t>hkb_1</t>
+  </si>
+  <si>
+    <t>hkb_2</t>
+  </si>
+  <si>
+    <t>hkb_3</t>
+  </si>
+  <si>
+    <t>hry_1</t>
+  </si>
+  <si>
+    <t>hry_2</t>
+  </si>
+  <si>
+    <t>kni_1</t>
+  </si>
+  <si>
+    <t>kni_2</t>
+  </si>
+  <si>
+    <t>kr_1</t>
+  </si>
+  <si>
+    <t>kr_2</t>
+  </si>
+  <si>
+    <t>mad_2</t>
+  </si>
+  <si>
+    <t>med_2</t>
+  </si>
+  <si>
+    <t>polII_H14</t>
+  </si>
+  <si>
+    <t>prd_1</t>
+  </si>
+  <si>
+    <t>prd_2</t>
+  </si>
+  <si>
+    <t>run_1</t>
+  </si>
+  <si>
+    <t>run_2</t>
+  </si>
+  <si>
+    <t>shn_2</t>
+  </si>
+  <si>
+    <t>shn_3</t>
+  </si>
+  <si>
+    <t>slp1_1</t>
+  </si>
+  <si>
+    <t>sna_1</t>
+  </si>
+  <si>
+    <t>sna_2</t>
+  </si>
+  <si>
+    <t>TFIIB_1</t>
+  </si>
+  <si>
+    <t>tll_1</t>
+  </si>
+  <si>
+    <t>twi_1</t>
+  </si>
+  <si>
+    <t>twi_2</t>
+  </si>
+  <si>
+    <t>A-P</t>
+  </si>
+  <si>
+    <t>early</t>
+  </si>
+  <si>
+    <t>maternal</t>
+  </si>
+  <si>
+    <t>gap-like</t>
+  </si>
+  <si>
+    <t>D-V</t>
+  </si>
+  <si>
+    <t>pair-rule</t>
+  </si>
+  <si>
+    <t>gap</t>
+  </si>
+  <si>
+    <t>terminal</t>
+  </si>
+  <si>
+    <t>zygotic</t>
   </si>
 </sst>
 </file>
@@ -1214,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N9"/>
+  <dimension ref="B1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1467,6 +1600,12 @@
       <c r="M9">
         <f>SUM(J9:L9)</f>
         <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <f>151/248</f>
+        <v>0.6088709677419355</v>
       </c>
     </row>
   </sheetData>
@@ -1564,4 +1703,790 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" t="s">
+        <v>71</v>
+      </c>
+      <c r="I30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" t="s">
+        <v>71</v>
+      </c>
+      <c r="I33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="F1:I35">
+    <sortCondition ref="G1:G35"/>
+    <sortCondition ref="I1:I35"/>
+    <sortCondition ref="F1:F35"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>